<commit_message>
Revert to 15 May 99e8d37f5ebf
</commit_message>
<xml_diff>
--- a/assets/Dev_evangelism_budget_v03_wm_2016.04.01.xlsx
+++ b/assets/Dev_evangelism_budget_v03_wm_2016.04.01.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilsonmar/gits/wilsonmar/wilsonmar.github.io/assets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6EF50D3D-43F3-054C-B829-5CBA43DA0C19}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22980" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="22980" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Tasks!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -38,6 +32,9 @@
     <t>Key resources / partners</t>
   </si>
   <si>
+    <t>Cities/regions target schedule</t>
+  </si>
+  <si>
     <t>Conferences to participate (sign up deadlines)</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
     <t>Note</t>
   </si>
   <si>
+    <t>Billing/insurance by MBO Partners in Virginia</t>
+  </si>
+  <si>
     <t>Meetups at cities</t>
   </si>
   <si>
@@ -144,22 +144,16 @@
   </si>
   <si>
     <t>Ext.</t>
-  </si>
-  <si>
-    <t>Cities/regions targets list</t>
-  </si>
-  <si>
-    <t>Billing/liab. Insurance by MBO Partners</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -253,7 +247,7 @@
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -287,14 +281,14 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="23">
@@ -327,9 +321,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -621,14 +612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -642,42 +633,42 @@
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="9"/>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -695,17 +686,17 @@
         <v>1.2578616352201257</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1">
       <c r="A3" s="9"/>
       <c r="B3" s="1"/>
       <c r="F3" s="4"/>
       <c r="G3" s="7"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -728,12 +719,12 @@
         <v>2.5157232704402515</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -754,12 +745,12 @@
         <v>1.8867924528301887</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10">
       <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -780,12 +771,12 @@
         <v>1.2578616352201257</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -806,9 +797,9 @@
         <v>1.8867924528301887</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -817,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E14" si="0">IF(A9&gt;0,D9*A9,D9)</f>
+        <f>IF(A9&gt;0,D9*A9,D9)</f>
         <v>7</v>
       </c>
       <c r="F9" s="5">
@@ -829,12 +820,12 @@
         <v>4.4025157232704402</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -843,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(A10&gt;0,D10*A10,D10)</f>
         <v>8</v>
       </c>
       <c r="F10" s="5">
@@ -855,12 +846,12 @@
         <v>5.0314465408805029</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -869,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(A11&gt;0,D11*A11,D11)</f>
         <v>3</v>
       </c>
       <c r="F11" s="5">
@@ -881,9 +872,9 @@
         <v>1.8867924528301887</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10">
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -892,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(A12&gt;0,D12*A12,D12)</f>
         <v>3</v>
       </c>
       <c r="F12" s="5">
@@ -904,9 +895,9 @@
         <v>1.8867924528301887</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10">
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -915,7 +906,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(A13&gt;0,D13*A13,D13)</f>
         <v>6</v>
       </c>
       <c r="F13" s="5">
@@ -927,12 +918,12 @@
         <v>3.7735849056603774</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -941,7 +932,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(A14&gt;0,D14*A14,D14)</f>
         <v>3</v>
       </c>
       <c r="F14" s="5">
@@ -953,12 +944,12 @@
         <v>1.8867924528301887</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -979,9 +970,9 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -1002,12 +993,12 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="A18" s="10">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>4</v>
@@ -1029,15 +1020,15 @@
         <v>3.7735849056603774</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="10">
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>4</v>
@@ -1059,12 +1050,12 @@
         <v>3.7735849056603774</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" s="10">
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -1085,9 +1076,9 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="B22" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
@@ -1108,12 +1099,12 @@
         <v>0.62893081761006286</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="10">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1135,12 +1126,12 @@
         <v>5.0314465408805029</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1161,12 +1152,12 @@
         <v>1.8867924528301887</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" s="10">
         <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" s="1">
         <v>5</v>
@@ -1188,13 +1179,13 @@
         <v>6.2893081761006284</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" s="11">
         <f>Totals!G2/5</f>
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D28" s="8">
         <f>A28*0.7</f>
@@ -1213,12 +1204,12 @@
         <v>5.2830188679245271</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" s="11">
         <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D29" s="8">
         <f>A29</f>
@@ -1237,7 +1228,7 @@
         <v>1.8867924528301887</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="F31" s="1"/>
     </row>
   </sheetData>
@@ -1313,19 +1304,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="7" max="7" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="str">
         <f>Tasks!A1</f>
         <v>#</v>
@@ -1367,7 +1358,7 @@
         <v>#</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" thickBot="1">
       <c r="D2" s="3">
         <f>SUM(Tasks!D1:D30)</f>
         <v>95.4</v>
@@ -1378,7 +1369,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:10" ht="15" thickTop="1"/>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
     <cfRule type="colorScale" priority="2">
@@ -1415,12 +1406,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>